<commit_message>
propgation bug fixed and evaluation data enhanced
</commit_message>
<xml_diff>
--- a/EvaluationData/Q4.2_AmountOfElements.xlsx
+++ b/EvaluationData/Q4.2_AmountOfElements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Desktop\Masterarbeit\UncertaintyImpactAnalysis\EvaluationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8EAE21-5E33-4F28-8477-1D97CCA12867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3F78EC-0408-49E6-A349-CB8695B64F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22830" yWindow="2220" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>